<commit_message>
added weird result examination
</commit_message>
<xml_diff>
--- a/GAP_comp_norm.xlsx
+++ b/GAP_comp_norm.xlsx
@@ -626,7 +626,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2">
-        <v>0.32895803451538086</v>
+        <v>0.3229990005493164</v>
       </c>
       <c r="B2">
         <v>0.0</v>
@@ -661,7 +661,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3">
-        <v>0.07312202453613281</v>
+        <v>0.12165498733520508</v>
       </c>
       <c r="B3">
         <v>0.0</v>
@@ -696,7 +696,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4">
-        <v>0.1360020637512207</v>
+        <v>0.11770105361938477</v>
       </c>
       <c r="B4">
         <v>0.0</v>
@@ -731,7 +731,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5">
-        <v>0.41185593605041504</v>
+        <v>0.40745019912719727</v>
       </c>
       <c r="B5">
         <v>0.0</v>
@@ -766,7 +766,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
-        <v>1.5002591609954834</v>
+        <v>1.6915290355682373</v>
       </c>
       <c r="B6">
         <v>0.0</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7">
-        <v>0.3257720470428467</v>
+        <v>0.2897801399230957</v>
       </c>
       <c r="B7">
         <v>0.0</v>
@@ -836,7 +836,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8">
-        <v>0.16146302223205566</v>
+        <v>0.17392897605895996</v>
       </c>
       <c r="B8">
         <v>0.0</v>
@@ -871,7 +871,7 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9">
-        <v>0.23634004592895508</v>
+        <v>0.2842140197753906</v>
       </c>
       <c r="B9">
         <v>0.0</v>
@@ -906,7 +906,7 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10">
-        <v>0.41988205909729004</v>
+        <v>0.43554091453552246</v>
       </c>
       <c r="B10">
         <v>0.0</v>
@@ -941,7 +941,7 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11">
-        <v>0.34295082092285156</v>
+        <v>0.35520219802856445</v>
       </c>
       <c r="B11">
         <v>0.0</v>
@@ -976,7 +976,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12">
-        <v>1.7649331092834473</v>
+        <v>1.7538189888000488</v>
       </c>
       <c r="B12">
         <v>0.0</v>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13">
-        <v>1.5600299835205078</v>
+        <v>1.6837728023529053</v>
       </c>
       <c r="B13">
         <v>0.0</v>
@@ -1046,7 +1046,7 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14">
-        <v>1.404716968536377</v>
+        <v>1.4518780708312988</v>
       </c>
       <c r="B14">
         <v>0.0</v>
@@ -1081,7 +1081,7 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15">
-        <v>8.153630018234253</v>
+        <v>8.470750093460083</v>
       </c>
       <c r="B15">
         <v>0.0</v>
@@ -1116,7 +1116,7 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16">
-        <v>2.374099016189575</v>
+        <v>2.408931016921997</v>
       </c>
       <c r="B16">
         <v>0.0</v>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17">
-        <v>286.6744978427887</v>
+        <v>284.300626039505</v>
       </c>
       <c r="B17">
         <v>0.0</v>
@@ -1186,7 +1186,7 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18">
-        <v>411.2340478897095</v>
+        <v>410.2300720214844</v>
       </c>
       <c r="B18">
         <v>0.0</v>
@@ -1221,19 +1221,19 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19">
-        <v>1500.2164039611816</v>
+        <v>3600.25691986084</v>
       </c>
       <c r="B19">
-        <v>0.00014310345696249841</v>
+        <v>0.000123033500004401</v>
       </c>
       <c r="C19">
-        <v>9326.00000000001</v>
+        <v>9326.000000000024</v>
       </c>
       <c r="D19" t="s">
         <v>32</v>
       </c>
       <c r="E19">
-        <v>0.00014310345696249841</v>
+        <v>0.000123033500004401</v>
       </c>
       <c r="F19" t="s">
         <v>12</v>
@@ -1251,12 +1251,12 @@
         <v>900</v>
       </c>
       <c r="K19">
-        <v>9326.00000000001</v>
+        <v>9326.000000000024</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20">
-        <v>74.62812805175781</v>
+        <v>75.52114486694336</v>
       </c>
       <c r="B20">
         <v>9.999957056182064e-5</v>
@@ -1291,19 +1291,19 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21">
-        <v>1501.3158030509949</v>
+        <v>1352.9148960113525</v>
       </c>
       <c r="B21">
-        <v>0.0001585770788202237</v>
+        <v>9.98685375930784e-5</v>
       </c>
       <c r="C21">
-        <v>17146.000000000047</v>
+        <v>17145.00000000003</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="E21">
-        <v>0.0001585770788202237</v>
+        <v>9.98685375930784e-5</v>
       </c>
       <c r="F21" t="s">
         <v>12</v>
@@ -1321,12 +1321,12 @@
         <v>1600</v>
       </c>
       <c r="K21">
-        <v>17146.000000000047</v>
+        <v>17145.00000000003</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22">
-        <v>1502.981850862503</v>
+        <v>3602.0627839565277</v>
       </c>
       <c r="B22">
         <v>0.00024559464603671487</v>
@@ -1361,7 +1361,7 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23">
-        <v>27.767214059829712</v>
+        <v>25.870085954666138</v>
       </c>
       <c r="B23">
         <v>0.0</v>
@@ -1396,19 +1396,19 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24">
-        <v>1500.0161771774292</v>
+        <v>3600.0179359912872</v>
       </c>
       <c r="B24">
-        <v>0.0012270907537236502</v>
+        <v>0.0005101364049129629</v>
       </c>
       <c r="C24">
-        <v>6350.0</v>
+        <v>6348.000000000327</v>
       </c>
       <c r="D24" t="s">
         <v>32</v>
       </c>
       <c r="E24">
-        <v>0.0012270907537236502</v>
+        <v>0.0005101364049129629</v>
       </c>
       <c r="F24" t="s">
         <v>12</v>
@@ -1426,24 +1426,24 @@
         <v>100</v>
       </c>
       <c r="K24">
-        <v>6350.0</v>
+        <v>6348.000000000327</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25">
-        <v>1504.155776977539</v>
+        <v>3608.315566778183</v>
       </c>
       <c r="B25">
-        <v>0.006433786334995149</v>
+        <v>0.006080916498046459</v>
       </c>
       <c r="C25">
-        <v>6209.0</v>
+        <v>6207.0</v>
       </c>
       <c r="D25" t="s">
         <v>32</v>
       </c>
       <c r="E25">
-        <v>0.006433786334995149</v>
+        <v>0.006080916498046459</v>
       </c>
       <c r="F25" t="s">
         <v>12</v>
@@ -1461,12 +1461,12 @@
         <v>100</v>
       </c>
       <c r="K25">
-        <v>6209.0</v>
+        <v>6207.0</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26">
-        <v>1177.0813059806824</v>
+        <v>1213.0529799461365</v>
       </c>
       <c r="B26">
         <v>0.0</v>
@@ -1501,19 +1501,19 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27">
-        <v>1501.5007100105286</v>
+        <v>3601.960891008377</v>
       </c>
       <c r="B27">
-        <v>0.0007677305445732689</v>
+        <v>0.0008286443327412408</v>
       </c>
       <c r="C27">
-        <v>12434.000000000015</v>
+        <v>12435.0</v>
       </c>
       <c r="D27" t="s">
         <v>32</v>
       </c>
       <c r="E27">
-        <v>0.0007677305445732689</v>
+        <v>0.0008286443327412408</v>
       </c>
       <c r="F27" t="s">
         <v>12</v>
@@ -1531,15 +1531,15 @@
         <v>200</v>
       </c>
       <c r="K27">
-        <v>12434.000000000015</v>
+        <v>12435.0</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28">
-        <v>1504.8537669181824</v>
+        <v>3604.9224960803986</v>
       </c>
       <c r="B28">
-        <v>0.0027577680525762644</v>
+        <v>0.002743763479497844</v>
       </c>
       <c r="C28">
         <v>12260.0</v>
@@ -1548,7 +1548,7 @@
         <v>32</v>
       </c>
       <c r="E28">
-        <v>0.0027577680525762644</v>
+        <v>0.002743763479497844</v>
       </c>
       <c r="F28" t="s">
         <v>12</v>
@@ -1571,19 +1571,19 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29">
-        <v>1503.4256219863892</v>
+        <v>3603.8255751132965</v>
       </c>
       <c r="B29">
-        <v>0.0005127835303233549</v>
+        <v>0.0004686373770336547</v>
       </c>
       <c r="C29">
-        <v>24970.99999997446</v>
+        <v>24970.0</v>
       </c>
       <c r="D29" t="s">
         <v>32</v>
       </c>
       <c r="E29">
-        <v>0.0005127835303233549</v>
+        <v>0.0004686373770336547</v>
       </c>
       <c r="F29" t="s">
         <v>12</v>
@@ -1601,24 +1601,24 @@
         <v>400</v>
       </c>
       <c r="K29">
-        <v>24970.99999997446</v>
+        <v>24970.0</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30">
-        <v>1502.9683170318604</v>
+        <v>3603.810455083847</v>
       </c>
       <c r="B30">
-        <v>0.0013459423234491257</v>
+        <v>0.0012089126022245004</v>
       </c>
       <c r="C30">
-        <v>24590.999999998417</v>
+        <v>24588.0</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
       </c>
       <c r="E30">
-        <v>0.0013459423234491257</v>
+        <v>0.0012089126022245004</v>
       </c>
       <c r="F30" t="s">
         <v>12</v>
@@ -1636,24 +1636,24 @@
         <v>400</v>
       </c>
       <c r="K30">
-        <v>24590.999999998417</v>
+        <v>24588.0</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31">
-        <v>1505.8376169204712</v>
+        <v>3605.4233560562134</v>
       </c>
       <c r="B31">
-        <v>0.004660098924907876</v>
+        <v>0.004375204448806894</v>
       </c>
       <c r="C31">
-        <v>24463.0</v>
+        <v>24456.0</v>
       </c>
       <c r="D31" t="s">
         <v>32</v>
       </c>
       <c r="E31">
-        <v>0.004660098924907876</v>
+        <v>0.004375204448806894</v>
       </c>
       <c r="F31" t="s">
         <v>12</v>
@@ -1671,24 +1671,24 @@
         <v>400</v>
       </c>
       <c r="K31">
-        <v>24463.0</v>
+        <v>24456.0</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32">
-        <v>1502.223294019699</v>
+        <v>3605.3445649147034</v>
       </c>
       <c r="B32">
-        <v>0.00034922788820991704</v>
+        <v>0.00033017274456214685</v>
       </c>
       <c r="C32">
-        <v>55420.99999999997</v>
+        <v>55420.00000000957</v>
       </c>
       <c r="D32" t="s">
         <v>32</v>
       </c>
       <c r="E32">
-        <v>0.00034922788820991704</v>
+        <v>0.00033017274456214685</v>
       </c>
       <c r="F32" t="s">
         <v>12</v>
@@ -1706,24 +1706,24 @@
         <v>900</v>
       </c>
       <c r="K32">
-        <v>55420.99999999997</v>
+        <v>55420.00000000957</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33">
-        <v>1502.888333082199</v>
+        <v>3602.5572600364685</v>
       </c>
       <c r="B33">
-        <v>0.0014899690768997635</v>
+        <v>0.0008888279143038277</v>
       </c>
       <c r="C33">
-        <v>54913.000000001004</v>
+        <v>54880.0</v>
       </c>
       <c r="D33" t="s">
         <v>32</v>
       </c>
       <c r="E33">
-        <v>0.0014899690768997635</v>
+        <v>0.0008888279143038277</v>
       </c>
       <c r="F33" t="s">
         <v>12</v>
@@ -1741,24 +1741,24 @@
         <v>900</v>
       </c>
       <c r="K33">
-        <v>54913.000000001004</v>
+        <v>54880.0</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34">
-        <v>1504.2819550037384</v>
+        <v>3607.351403951645</v>
       </c>
       <c r="B34">
-        <v>0.0033434428326082114</v>
+        <v>0.003379859690148674</v>
       </c>
       <c r="C34">
-        <v>54734.0</v>
+        <v>54736.0</v>
       </c>
       <c r="D34" t="s">
         <v>32</v>
       </c>
       <c r="E34">
-        <v>0.0033434428326082114</v>
+        <v>0.003379859690148674</v>
       </c>
       <c r="F34" t="s">
         <v>12</v>
@@ -1776,24 +1776,24 @@
         <v>900</v>
       </c>
       <c r="K34">
-        <v>54734.0</v>
+        <v>54736.0</v>
       </c>
     </row>
     <row r="35" spans="1:11">
       <c r="A35">
-        <v>1501.6598711013794</v>
+        <v>3604.7848250865936</v>
       </c>
       <c r="B35">
-        <v>0.00036664157350583507</v>
+        <v>0.0003357184650025423</v>
       </c>
       <c r="C35">
-        <v>97858.0</v>
+        <v>97855.0</v>
       </c>
       <c r="D35" t="s">
         <v>32</v>
       </c>
       <c r="E35">
-        <v>0.00036664157350583507</v>
+        <v>0.0003357184650025423</v>
       </c>
       <c r="F35" t="s">
         <v>12</v>
@@ -1811,24 +1811,24 @@
         <v>1600</v>
       </c>
       <c r="K35">
-        <v>97858.0</v>
+        <v>97855.0</v>
       </c>
     </row>
     <row r="36" spans="1:11">
       <c r="A36">
-        <v>1504.6499741077423</v>
+        <v>3607.671318054199</v>
       </c>
       <c r="B36">
-        <v>0.00143966270759392</v>
+        <v>0.0014499311025643292</v>
       </c>
       <c r="C36">
-        <v>97245.0</v>
+        <v>97246.0</v>
       </c>
       <c r="D36" t="s">
         <v>32</v>
       </c>
       <c r="E36">
-        <v>0.00143966270759392</v>
+        <v>0.0014499311025643292</v>
       </c>
       <c r="F36" t="s">
         <v>12</v>
@@ -1846,24 +1846,24 @@
         <v>1600</v>
       </c>
       <c r="K36">
-        <v>97245.0</v>
+        <v>97246.0</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37">
-        <v>1502.641625881195</v>
+        <v>3607.0605511665344</v>
       </c>
       <c r="B37">
-        <v>0.0021595162683543897</v>
+        <v>0.002138993439047472</v>
       </c>
       <c r="C37">
-        <v>97244.0</v>
+        <v>97242.0</v>
       </c>
       <c r="D37" t="s">
         <v>32</v>
       </c>
       <c r="E37">
-        <v>0.0021595162683543897</v>
+        <v>0.002138993439047472</v>
       </c>
       <c r="F37" t="s">
         <v>12</v>
@@ -1881,12 +1881,12 @@
         <v>1600</v>
       </c>
       <c r="K37">
-        <v>97244.0</v>
+        <v>97242.0</v>
       </c>
     </row>
     <row r="38" spans="1:11">
       <c r="A38">
-        <v>1.2023727893829346</v>
+        <v>2.037170886993408</v>
       </c>
       <c r="B38">
         <v>9.97576943777629e-5</v>
@@ -1921,7 +1921,7 @@
     </row>
     <row r="39" spans="1:11">
       <c r="A39">
-        <v>3.8723559379577637</v>
+        <v>8.591979026794434</v>
       </c>
       <c r="B39">
         <v>9.998499614844937e-5</v>
@@ -1956,7 +1956,7 @@
     </row>
     <row r="40" spans="1:11">
       <c r="A40">
-        <v>6.966852903366089</v>
+        <v>8.96023416519165</v>
       </c>
       <c r="B40">
         <v>0.0</v>
@@ -1991,7 +1991,7 @@
     </row>
     <row r="41" spans="1:11">
       <c r="A41">
-        <v>1.1684949398040771</v>
+        <v>1.3177781105041504</v>
       </c>
       <c r="B41">
         <v>7.96359677226796e-5</v>
@@ -2026,7 +2026,7 @@
     </row>
     <row r="42" spans="1:11">
       <c r="A42">
-        <v>6.0121800899505615</v>
+        <v>11.044636964797974</v>
       </c>
       <c r="B42">
         <v>9.999829327606199e-5</v>
@@ -2061,7 +2061,7 @@
     </row>
     <row r="43" spans="1:11">
       <c r="A43">
-        <v>4.8368239402771</v>
+        <v>6.7002809047698975</v>
       </c>
       <c r="B43">
         <v>6.831845691835766e-5</v>
@@ -2096,7 +2096,7 @@
     </row>
     <row r="44" spans="1:11">
       <c r="A44">
-        <v>9.62270212173462</v>
+        <v>10.944949865341187</v>
       </c>
       <c r="B44">
         <v>9.166646451921332e-5</v>
@@ -2131,7 +2131,7 @@
     </row>
     <row r="45" spans="1:11">
       <c r="A45">
-        <v>6.213791131973267</v>
+        <v>9.37498688697815</v>
       </c>
       <c r="B45">
         <v>3.580451099844054e-5</v>
@@ -2166,7 +2166,7 @@
     </row>
     <row r="46" spans="1:11">
       <c r="A46">
-        <v>159.83819818496704</v>
+        <v>184.60556602478027</v>
       </c>
       <c r="B46">
         <v>9.545596707633623e-5</v>
@@ -2201,7 +2201,7 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47">
-        <v>4.028379917144775</v>
+        <v>3.841671943664551</v>
       </c>
       <c r="B47">
         <v>9.823352220165787e-5</v>
@@ -2236,7 +2236,7 @@
     </row>
     <row r="48" spans="1:11">
       <c r="A48">
-        <v>15.982394933700562</v>
+        <v>18.37431001663208</v>
       </c>
       <c r="B48">
         <v>8.304912572602551e-5</v>
@@ -2271,7 +2271,7 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49">
-        <v>308.76006293296814</v>
+        <v>333.44506096839905</v>
       </c>
       <c r="B49">
         <v>9.995535898346713e-5</v>
@@ -2306,7 +2306,7 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50">
-        <v>23.676949977874756</v>
+        <v>24.974233150482178</v>
       </c>
       <c r="B50">
         <v>9.735487929124363e-5</v>
@@ -2341,7 +2341,7 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51">
-        <v>37.24802899360657</v>
+        <v>40.21325898170471</v>
       </c>
       <c r="B51">
         <v>8.125108610936504e-5</v>
@@ -2376,7 +2376,7 @@
     </row>
     <row r="52" spans="1:11">
       <c r="A52">
-        <v>241.64468789100647</v>
+        <v>250.65193891525269</v>
       </c>
       <c r="B52">
         <v>9.967714303255963e-5</v>

</xml_diff>